<commit_message>
add to the todo
</commit_message>
<xml_diff>
--- a/ProjectTODO.xlsx
+++ b/ProjectTODO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjh\Desktop\SE2\food-truck-project-group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler Ross\food-truck-project-group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E93740F-B92A-418A-97E4-FD0359D277FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CFCB15-4304-4EB3-8B9D-3607027BEF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB41F5DD-21FB-4C11-9406-0AB1034EB211}"/>
+    <workbookView xWindow="1065" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{EB41F5DD-21FB-4C11-9406-0AB1034EB211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>General</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Implement separate backend calls for editTruck/Account, dashboardData, etc. (for modularity)</t>
+  </si>
+  <si>
+    <t>Be able to unsubscribe from trucks</t>
   </si>
 </sst>
 </file>
@@ -561,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AA4CC5-2A25-409B-AFF7-6C8F7A4172DE}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,6 +785,11 @@
         <v>49</v>
       </c>
     </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
     </row>

</xml_diff>

<commit_message>
updated TODO excel sheet
</commit_message>
<xml_diff>
--- a/ProjectTODO.xlsx
+++ b/ProjectTODO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler Ross\food-truck-project-group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjh\Desktop\SE2\food-truck-project-group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CFCB15-4304-4EB3-8B9D-3607027BEF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65CB95D-AC78-4A40-B67B-89196D8D18D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{EB41F5DD-21FB-4C11-9406-0AB1034EB211}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB41F5DD-21FB-4C11-9406-0AB1034EB211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>General</t>
   </si>
@@ -45,21 +45,12 @@
     <t>Optional</t>
   </si>
   <si>
-    <t>Submitting in all places should redirect/refresh</t>
-  </si>
-  <si>
     <t>Maps (nearby trucks) needs implementation (on dashboard)</t>
   </si>
   <si>
-    <t xml:space="preserve">     If not logged (i.e. guest user), clicking dashboard says you can't (may redirect to login page)</t>
-  </si>
-  <si>
     <t>Cosmetic</t>
   </si>
   <si>
-    <t>Implement drop down menus for rating (preferences)</t>
-  </si>
-  <si>
     <t>Display stars for viewing (maybe setting) ratings)</t>
   </si>
   <si>
@@ -75,9 +66,6 @@
     <t xml:space="preserve">    (change front end accordingly)</t>
   </si>
   <si>
-    <t>No longer hardcode access to user dash - gain access via token (only /dashboard)</t>
-  </si>
-  <si>
     <t>Token should no longer be user's Id (for security)</t>
   </si>
   <si>
@@ -90,12 +78,6 @@
     <t>On "signup" shouldn't redirect to /login but rather to /dashboard (with appropriate token set)</t>
   </si>
   <si>
-    <t>Setting the user type doesn't work - fix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Customer/guest shouldn't have access to "create food truck"</t>
-  </si>
-  <si>
     <t>Any time there is some kind of submission, JS alert should trigger to inform user</t>
   </si>
   <si>
@@ -123,9 +105,6 @@
     <t>Make sure regex are enforced where appropriate (such as numerical entry fields)</t>
   </si>
   <si>
-    <t>If user enters invalid address &amp; submits, they are alerted instead of posting</t>
-  </si>
-  <si>
     <t>If frontend ever gets something NULL from back end, make sure it handles correctly</t>
   </si>
   <si>
@@ -165,9 +144,6 @@
     <t>Remove some unnecessary code</t>
   </si>
   <si>
-    <t>No log out option???</t>
-  </si>
-  <si>
     <t>Need checks for existing username/email before creating account/changing username</t>
   </si>
   <si>
@@ -186,13 +162,19 @@
     <t>Can't find MapComponent on my dashboard end (for now don't enter address)</t>
   </si>
   <si>
-    <t>Food type preferences should have existing value be default on dashboard</t>
-  </si>
-  <si>
     <t>Implement separate backend calls for editTruck/Account, dashboardData, etc. (for modularity)</t>
   </si>
   <si>
     <t>Be able to unsubscribe from trucks</t>
+  </si>
+  <si>
+    <t>Customer/guest shouldn't have access to "create food truck"</t>
+  </si>
+  <si>
+    <t>Submitting in all places should redirect/refresh - particularly subscribe, createTruck, edit, etc.</t>
+  </si>
+  <si>
+    <t>If user enters invalid address &amp; submits, they are alerted</t>
   </si>
 </sst>
 </file>
@@ -564,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AA4CC5-2A25-409B-AFF7-6C8F7A4172DE}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -591,123 +573,126 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>50</v>
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,72 +707,37 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
+      <c r="A16" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
+      <c r="A17" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
+      <c r="A18" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>31</v>
+      <c r="A19" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
+      <c r="A20" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New backend calls; can now: Delete food truck, delete location from truck's route list, delete food item from menu Can get a user's subscribed food trucks & ratings (for display on userdetails page) User can now unsubscribe from food truck Minor fixes/revisions
</commit_message>
<xml_diff>
--- a/ProjectTODO.xlsx
+++ b/ProjectTODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjh\Desktop\SE2\food-truck-project-group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65CB95D-AC78-4A40-B67B-89196D8D18D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C9C7DF-5249-4D14-AEAD-667B0A55E493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB41F5DD-21FB-4C11-9406-0AB1034EB211}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>General</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Make sure unique emails are enforced at all times in backend</t>
   </si>
   <si>
-    <t>Deleting:</t>
-  </si>
-  <si>
     <t>Have Owner extend Customer (&amp; have list of food trucks; is this compatible w/Hibernate SQL?</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Implement separate backend calls for editTruck/Account, dashboardData, etc. (for modularity)</t>
   </si>
   <si>
-    <t>Be able to unsubscribe from trucks</t>
-  </si>
-  <si>
     <t>Customer/guest shouldn't have access to "create food truck"</t>
   </si>
   <si>
@@ -175,6 +169,15 @@
   </si>
   <si>
     <t>If user enters invalid address &amp; submits, they are alerted</t>
+  </si>
+  <si>
+    <t>Deleting: (implemented in backend - now just need front end to handle)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     (implemented in backend - now just need front end to handle)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Be able to unsubscribe from trucks</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +576,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -596,21 +599,21 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,13 +621,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,24 +635,24 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -657,10 +660,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,18 +671,18 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,52 +695,57 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
+      <c r="A16" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>36</v>
+      <c r="A17" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
+      <c r="A18" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bug fixes, including telling a user if they can't use an email when signing up. Also removed "Add rating" from editTruck bc it was an old debugging feature and is now unnecessary
</commit_message>
<xml_diff>
--- a/ProjectTODO.xlsx
+++ b/ProjectTODO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjh\Desktop\SE2\food-truck-project-group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjh\Desktop\SE2\Project\food-truck-project-group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C9C7DF-5249-4D14-AEAD-667B0A55E493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5B896A-5D35-49FA-924A-3C2FD5292026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB41F5DD-21FB-4C11-9406-0AB1034EB211}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>General</t>
   </si>
@@ -60,30 +60,18 @@
     <t>Front end needs to handle error messages &amp; inform client (e.g. "not found" or "failed to log in")</t>
   </si>
   <si>
-    <t xml:space="preserve">    (rather than wrapping in "Preferences", "JSONWrapper", etc.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (change front end accordingly)</t>
-  </si>
-  <si>
     <t>Token should no longer be user's Id (for security)</t>
   </si>
   <si>
     <t>Fix haphazardly thrown together "nearby trucks" on dash</t>
   </si>
   <si>
-    <t>Display current preferences on dash (including all food type preferences)</t>
-  </si>
-  <si>
     <t>On "signup" shouldn't redirect to /login but rather to /dashboard (with appropriate token set)</t>
   </si>
   <si>
     <t>Any time there is some kind of submission, JS alert should trigger to inform user</t>
   </si>
   <si>
-    <t>Make sure unique emails are enforced at all times in backend</t>
-  </si>
-  <si>
     <t>Have Owner extend Customer (&amp; have list of food trucks; is this compatible w/Hibernate SQL?</t>
   </si>
   <si>
@@ -123,45 +111,21 @@
     <t>Handle case where user enters a userid or truckid (in URL) that does not exist</t>
   </si>
   <si>
-    <t>Implement userDetails to just look at the details of other users (such as their ratings)</t>
-  </si>
-  <si>
-    <t>Dashboard shouldn't send preference change to backend if it wasn't set by user (e.g. null)</t>
-  </si>
-  <si>
     <t>"Route" not displaying on truckDetails</t>
   </si>
   <si>
-    <t>Remove "set rating preference" on editTruck</t>
-  </si>
-  <si>
     <t>Stateful design</t>
   </si>
   <si>
     <t>Remove some unnecessary code</t>
   </si>
   <si>
-    <t>Need checks for existing username/email before creating account/changing username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     I know there wasn't a check when I created a new test one when one with same uname existed</t>
-  </si>
-  <si>
-    <t>Either access "editAccount" (&amp; ability to change username/password from it)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    or modify dashboard to have same functionality</t>
-  </si>
-  <si>
     <t>NullPtrException on finding nearest trucks</t>
   </si>
   <si>
     <t>Can't find MapComponent on my dashboard end (for now don't enter address)</t>
   </si>
   <si>
-    <t>Implement separate backend calls for editTruck/Account, dashboardData, etc. (for modularity)</t>
-  </si>
-  <si>
     <t>Customer/guest shouldn't have access to "create food truck"</t>
   </si>
   <si>
@@ -172,12 +136,6 @@
   </si>
   <si>
     <t>Deleting: (implemented in backend - now just need front end to handle)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     (implemented in backend - now just need front end to handle)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Be able to unsubscribe from trucks</t>
   </si>
 </sst>
 </file>
@@ -550,7 +508,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +534,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -585,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,157 +554,102 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>42</v>
+      <c r="A10" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A12" s="3"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A19" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>

</xml_diff>